<commit_message>
update timesheet feature 7.24
</commit_message>
<xml_diff>
--- a/BE/API/wwwroot/Timesheet/base.xlsx
+++ b/BE/API/wwwroot/Timesheet/base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C721B27-0273-4ABD-883A-F3F2EB44B429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6118F99-4183-4545-8F61-CC8C2FC782C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -846,7 +846,7 @@
   <dimension ref="B1:AJ22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:AJ1"/>
+      <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="7" spans="2:36" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="39">
-        <v>11111</v>
+        <v>202207237495</v>
       </c>
       <c r="C7" s="40"/>
       <c r="D7" s="41" t="s">
@@ -1168,79 +1168,79 @@
         <v>0</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="W7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="R7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="S7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="T7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="U7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="V7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="W7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="X7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="AC7" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AD7" s="4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE7" s="4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF7" s="4" t="s">
         <v>0</v>
@@ -1252,7 +1252,7 @@
         <v>0</v>
       </c>
       <c r="AI7" s="4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AJ7" s="4" t="s">
         <v>7</v>
@@ -1271,16 +1271,16 @@
         <v>6</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>0</v>
@@ -1292,16 +1292,16 @@
         <v>0</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R8" s="4" t="s">
         <v>0</v>
@@ -1313,16 +1313,16 @@
         <v>0</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V8" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W8" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X8" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y8" s="5" t="s">
         <v>0</v>
@@ -1334,16 +1334,16 @@
         <v>0</v>
       </c>
       <c r="AB8" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AC8" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AD8" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE8" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF8" s="5" t="s">
         <v>0</v>
@@ -1355,7 +1355,7 @@
         <v>0</v>
       </c>
       <c r="AI8" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AJ8" s="5" t="s">
         <v>7</v>
@@ -1374,16 +1374,16 @@
         <v>6</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1395,16 +1395,16 @@
         <v>0</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R9" s="4" t="s">
         <v>0</v>
@@ -1416,16 +1416,16 @@
         <v>0</v>
       </c>
       <c r="U9" s="4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V9" s="4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W9" s="4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X9" s="4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y9" s="4" t="s">
         <v>0</v>
@@ -1437,16 +1437,16 @@
         <v>0</v>
       </c>
       <c r="AB9" s="4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AC9" s="4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AD9" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AE9" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AF9" s="4" t="s">
         <v>5</v>
@@ -1458,7 +1458,7 @@
         <v>1</v>
       </c>
       <c r="AI9" s="4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AJ9" s="4" t="s">
         <v>7</v>
@@ -1477,16 +1477,16 @@
         <v>0</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>0</v>
@@ -1498,16 +1498,16 @@
         <v>0</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R10" s="5" t="s">
         <v>0</v>
@@ -1519,16 +1519,16 @@
         <v>0</v>
       </c>
       <c r="U10" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V10" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W10" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X10" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y10" s="5" t="s">
         <v>0</v>
@@ -1540,16 +1540,16 @@
         <v>0</v>
       </c>
       <c r="AB10" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AC10" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AD10" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE10" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF10" s="5" t="s">
         <v>0</v>
@@ -1561,7 +1561,7 @@
         <v>0</v>
       </c>
       <c r="AI10" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AJ10" s="5" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
update pay feature 7.24
</commit_message>
<xml_diff>
--- a/BE/API/wwwroot/Timesheet/base.xlsx
+++ b/BE/API/wwwroot/Timesheet/base.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VisuaStudio\HR_Management\New\HR-Management\BE\API\wwwroot\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6118F99-4183-4545-8F61-CC8C2FC782C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFCA3672-43A6-4E3E-8D8C-90F70DAEBD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="26">
   <si>
     <t>W</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Huong</t>
+  </si>
+  <si>
+    <t>202207237495</t>
   </si>
 </sst>
 </file>
@@ -308,7 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -363,11 +366,38 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -381,6 +411,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -393,64 +429,37 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -846,7 +855,7 @@
   <dimension ref="B1:AJ22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AA8" sqref="AA8"/>
+      <selection activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,43 +899,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:36" s="6" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
-      <c r="AG1" s="21"/>
-      <c r="AH1" s="21"/>
-      <c r="AI1" s="21"/>
-      <c r="AJ1" s="21"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="36"/>
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="36"/>
     </row>
     <row r="2" spans="2:36" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
@@ -951,86 +960,86 @@
       <c r="F3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="32"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="41"/>
       <c r="J3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="26"/>
-      <c r="L3" s="32"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="41"/>
       <c r="N3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="26"/>
-      <c r="P3" s="32"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="41"/>
       <c r="R3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="S3" s="26"/>
-      <c r="T3" s="27"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="38"/>
       <c r="V3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="W3" s="26"/>
-      <c r="X3" s="27"/>
+      <c r="W3" s="37"/>
+      <c r="X3" s="38"/>
       <c r="Z3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="AA3" s="26"/>
-      <c r="AB3" s="27"/>
+      <c r="AA3" s="37"/>
+      <c r="AB3" s="38"/>
       <c r="AD3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="26"/>
-      <c r="AF3" s="27"/>
+      <c r="AE3" s="37"/>
+      <c r="AF3" s="38"/>
     </row>
     <row r="4" spans="2:36" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="J4" s="46" t="s">
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="J4" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="N4" s="47" t="s">
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="N4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="R4" s="48" t="s">
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="R4" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="S4" s="48"/>
-      <c r="T4" s="48"/>
-      <c r="V4" s="49" t="s">
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="V4" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="W4" s="49"/>
-      <c r="X4" s="49"/>
-      <c r="Z4" s="43" t="s">
+      <c r="W4" s="26"/>
+      <c r="X4" s="26"/>
+      <c r="Z4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="AA4" s="43"/>
-      <c r="AB4" s="43"/>
-      <c r="AD4" s="44" t="s">
+      <c r="AA4" s="20"/>
+      <c r="AB4" s="20"/>
+      <c r="AD4" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AE4" s="44"/>
-      <c r="AF4" s="44"/>
+      <c r="AE4" s="21"/>
+      <c r="AF4" s="21"/>
     </row>
     <row r="5" spans="2:36" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:36" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="28" t="s">
+      <c r="C6" s="40"/>
+      <c r="D6" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="29"/>
+      <c r="E6" s="40"/>
       <c r="F6" s="2">
         <v>1</v>
       </c>
@@ -1156,14 +1165,14 @@
       </c>
     </row>
     <row r="7" spans="2:36" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="39">
-        <v>202207237495</v>
-      </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="41" t="s">
+      <c r="B7" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="42"/>
+      <c r="D7" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="42"/>
+      <c r="E7" s="28"/>
       <c r="F7" s="4" t="s">
         <v>0</v>
       </c>
@@ -1259,14 +1268,14 @@
       </c>
     </row>
     <row r="8" spans="2:36" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="30">
+      <c r="B8" s="45">
         <v>22222</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="33" t="s">
+      <c r="C8" s="46"/>
+      <c r="D8" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="34"/>
+      <c r="E8" s="30"/>
       <c r="F8" s="5" t="s">
         <v>6</v>
       </c>
@@ -1304,7 +1313,7 @@
         <v>3</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S8" s="5" t="s">
         <v>0</v>
@@ -1331,7 +1340,7 @@
         <v>0</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AB8" s="5" t="s">
         <v>0</v>
@@ -1362,14 +1371,14 @@
       </c>
     </row>
     <row r="9" spans="2:36" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="39">
+      <c r="B9" s="47">
         <v>33333</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="41" t="s">
+      <c r="C9" s="44"/>
+      <c r="D9" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="42"/>
+      <c r="E9" s="28"/>
       <c r="F9" s="4" t="s">
         <v>6</v>
       </c>
@@ -1410,7 +1419,7 @@
         <v>0</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T9" s="4" t="s">
         <v>0</v>
@@ -1465,14 +1474,14 @@
       </c>
     </row>
     <row r="10" spans="2:36" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="30">
+      <c r="B10" s="45">
         <v>44444</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="33" t="s">
+      <c r="C10" s="46"/>
+      <c r="D10" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="34"/>
+      <c r="E10" s="30"/>
       <c r="F10" s="5" t="s">
         <v>0</v>
       </c>
@@ -1489,7 +1498,7 @@
         <v>3</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>0</v>
@@ -1534,7 +1543,7 @@
         <v>0</v>
       </c>
       <c r="Z10" s="5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA10" s="5" t="s">
         <v>0</v>
@@ -1568,10 +1577,10 @@
       </c>
     </row>
     <row r="11" spans="2:36" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="37"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="25"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="34"/>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
       <c r="H11" s="18"/>
@@ -1605,10 +1614,10 @@
       <c r="AJ11" s="18"/>
     </row>
     <row r="12" spans="2:36" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="35"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
@@ -1642,10 +1651,10 @@
       <c r="AJ12" s="19"/>
     </row>
     <row r="13" spans="2:36" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="37"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="25"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="34"/>
       <c r="F13" s="18"/>
       <c r="G13" s="18"/>
       <c r="H13" s="18"/>
@@ -1679,10 +1688,10 @@
       <c r="AJ13" s="18"/>
     </row>
     <row r="14" spans="2:36" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="35"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="23"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="32"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
@@ -1716,10 +1725,10 @@
       <c r="AJ14" s="19"/>
     </row>
     <row r="15" spans="2:36" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="37"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="34"/>
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
       <c r="H15" s="18"/>
@@ -1753,10 +1762,10 @@
       <c r="AJ15" s="18"/>
     </row>
     <row r="16" spans="2:36" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="35"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="23"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="32"/>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
@@ -1790,10 +1799,10 @@
       <c r="AJ16" s="19"/>
     </row>
     <row r="17" spans="2:36" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="37"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="25"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="34"/>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
@@ -1827,10 +1836,10 @@
       <c r="AJ17" s="18"/>
     </row>
     <row r="18" spans="2:36" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="35"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="23"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="32"/>
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
@@ -1864,10 +1873,10 @@
       <c r="AJ18" s="19"/>
     </row>
     <row r="19" spans="2:36" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="37"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="34"/>
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
       <c r="H19" s="18"/>
@@ -1901,10 +1910,10 @@
       <c r="AJ19" s="18"/>
     </row>
     <row r="20" spans="2:36" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="35"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="23"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="32"/>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
@@ -1938,10 +1947,10 @@
       <c r="AJ20" s="19"/>
     </row>
     <row r="21" spans="2:36" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="37"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="34"/>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
       <c r="H21" s="18"/>
@@ -1975,10 +1984,10 @@
       <c r="AJ21" s="18"/>
     </row>
     <row r="22" spans="2:36" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="35"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="23"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="32"/>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
@@ -2013,39 +2022,6 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="AD4:AF4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
     <mergeCell ref="B1:AJ1"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E19"/>
@@ -2062,6 +2038,39 @@
     <mergeCell ref="S3:T3"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="AD4:AF4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="V4:X4"/>
   </mergeCells>
   <conditionalFormatting sqref="F7:AJ22">
     <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="V">

</xml_diff>